<commit_message>
Auto stash before merge of 'develop' and 'origin/develop'
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/06_upscale_almeria_NEW.xlsx
+++ b/backend_tests/z_input_files/v2/06_upscale_almeria_NEW.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="204">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -737,7 +737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -775,10 +775,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -957,7 +953,7 @@
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1979,8 +1975,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2002,7 +1998,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="20" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
@@ -3052,7 +3048,7 @@
       <c r="P26" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="Q26" s="10" t="s">
+      <c r="Q26" s="5" t="s">
         <v>129</v>
       </c>
       <c r="R26" s="7" t="s">
@@ -3577,9 +3573,7 @@
       <c r="J40" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K40" s="0" t="s">
-        <v>141</v>
-      </c>
+      <c r="K40" s="0"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
@@ -3684,9 +3678,7 @@
       <c r="J43" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="K43" s="0" t="s">
-        <v>141</v>
-      </c>
+      <c r="K43" s="0"/>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
@@ -3753,9 +3745,6 @@
       </c>
       <c r="J46" s="0" t="n">
         <v>0.6</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>141</v>
       </c>
       <c r="Q46" s="0" t="n">
         <v>2015</v>
@@ -4100,7 +4089,7 @@
       <c r="E7" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="10" t="n">
         <v>0.15</v>
       </c>
     </row>
@@ -4120,7 +4109,7 @@
       <c r="E8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="10" t="n">
         <v>0.19</v>
       </c>
     </row>
@@ -4140,7 +4129,7 @@
       <c r="E9" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="11" t="n">
+      <c r="F9" s="10" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -4160,7 +4149,7 @@
       <c r="E10" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="F10" s="10" t="n">
         <v>0.06</v>
       </c>
     </row>
@@ -4180,7 +4169,7 @@
       <c r="E11" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" s="11" t="n">
         <v>0.85</v>
       </c>
     </row>
@@ -4200,7 +4189,7 @@
       <c r="E12" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="12" t="n">
+      <c r="F12" s="11" t="n">
         <v>0.77</v>
       </c>
     </row>
@@ -4220,7 +4209,7 @@
       <c r="E13" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="12" t="n">
+      <c r="F13" s="11" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -4240,7 +4229,7 @@
       <c r="E14" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="11" t="n">
+      <c r="F14" s="10" t="n">
         <v>0.87</v>
       </c>
     </row>
@@ -4260,7 +4249,7 @@
       <c r="E15" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="F15" s="10" t="n">
         <v>0.94</v>
       </c>
     </row>
@@ -4280,7 +4269,7 @@
       <c r="E16" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="11" t="n">
+      <c r="F16" s="10" t="n">
         <v>0.04</v>
       </c>
     </row>
@@ -4300,7 +4289,7 @@
       <c r="E17" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="11" t="n">
+      <c r="F17" s="10" t="n">
         <v>0.92</v>
       </c>
     </row>
@@ -4320,7 +4309,7 @@
       <c r="E18" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="11" t="n">
+      <c r="F18" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4340,7 +4329,7 @@
       <c r="E19" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="F19" s="10" t="n">
         <v>0.13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improving outputs generation plus solved bug in Processor "clone()"
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/06_upscale_almeria_NEW.xlsx
+++ b/backend_tests/z_input_files/v2/06_upscale_almeria_NEW.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="204">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -737,7 +737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -778,10 +778,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -792,12 +788,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -944,8 +940,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -957,7 +953,7 @@
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1374,8 +1370,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1669,8 +1665,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1900,8 +1896,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1966,8 +1962,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1979,8 +1975,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2002,7 +1998,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="20" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
@@ -3052,7 +3048,7 @@
       <c r="P26" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="Q26" s="10" t="s">
+      <c r="Q26" s="5" t="s">
         <v>129</v>
       </c>
       <c r="R26" s="7" t="s">
@@ -3577,9 +3573,7 @@
       <c r="J40" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K40" s="0" t="s">
-        <v>141</v>
-      </c>
+      <c r="K40" s="0"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
@@ -3684,9 +3678,7 @@
       <c r="J43" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="K43" s="0" t="s">
-        <v>141</v>
-      </c>
+      <c r="K43" s="0"/>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
@@ -3754,9 +3746,6 @@
       <c r="J46" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="K46" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="Q46" s="0" t="n">
         <v>2015</v>
       </c>
@@ -3936,8 +3925,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4100,7 +4089,7 @@
       <c r="E7" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="10" t="n">
         <v>0.15</v>
       </c>
     </row>
@@ -4120,7 +4109,7 @@
       <c r="E8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="10" t="n">
         <v>0.19</v>
       </c>
     </row>
@@ -4140,7 +4129,7 @@
       <c r="E9" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="11" t="n">
+      <c r="F9" s="10" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -4160,7 +4149,7 @@
       <c r="E10" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="F10" s="10" t="n">
         <v>0.06</v>
       </c>
     </row>
@@ -4180,7 +4169,7 @@
       <c r="E11" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" s="11" t="n">
         <v>0.85</v>
       </c>
     </row>
@@ -4200,7 +4189,7 @@
       <c r="E12" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="12" t="n">
+      <c r="F12" s="11" t="n">
         <v>0.77</v>
       </c>
     </row>
@@ -4220,7 +4209,7 @@
       <c r="E13" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="12" t="n">
+      <c r="F13" s="11" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -4240,7 +4229,7 @@
       <c r="E14" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="11" t="n">
+      <c r="F14" s="10" t="n">
         <v>0.87</v>
       </c>
     </row>
@@ -4260,7 +4249,7 @@
       <c r="E15" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="F15" s="10" t="n">
         <v>0.94</v>
       </c>
     </row>
@@ -4280,7 +4269,7 @@
       <c r="E16" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="11" t="n">
+      <c r="F16" s="10" t="n">
         <v>0.04</v>
       </c>
     </row>
@@ -4300,7 +4289,7 @@
       <c r="E17" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="11" t="n">
+      <c r="F17" s="10" t="n">
         <v>0.92</v>
       </c>
     </row>
@@ -4320,7 +4309,7 @@
       <c r="E18" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="11" t="n">
+      <c r="F18" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4340,7 +4329,7 @@
       <c r="E19" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="F19" s="10" t="n">
         <v>0.13</v>
       </c>
     </row>
@@ -4349,8 +4338,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>